<commit_message>
fixed errors in json formatting
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1327" documentId="8_{DF39C3F4-3D1F-4401-A869-CC4FEA15FC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E67DD8-E389-49A2-A147-8A980958DDE5}"/>
+  <xr:revisionPtr revIDLastSave="1329" documentId="8_{DF39C3F4-3D1F-4401-A869-CC4FEA15FC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC67EF8E-8A76-4D89-9E23-4D45A8563597}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="27770" windowHeight="17640" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="27770" windowHeight="17640" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
@@ -1196,91 +1196,91 @@
     <t>Multi-Stage FIA</t>
   </si>
   <si>
-    <t>{"class":"ADC","sub_class”":"SAR","sub_sub_class","NS-SAR","performance":{"source":"measured","tech":"40","fs":"10e6","OSR":"8","SNDR_nyq":"83.8","SFDR_nyq":"94.3","P_nyq":"107e-6"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"100e6","OSR":"1","SNDR_nyq":"71.7","SFDR_nyq":"87.2","P_nyq":"0.7e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"1e9","OSR":"1","SNDR_nyq":"59.5","SFDR_nyq":"75.9","P_nyq":"10.9e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"40e6","OSR":"1","SNDR_nyq":"75.7","SFDR_nyq":"81.4","P_nyq":"8.21e-4"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"4e9","OSR":"1","SNDR_nyq":"61.9","SFDR_nyq":"75.2","P_nyq":"75e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"75.5","SFDR_nyq":"62.3","P_nyq":"2.8e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"200e6","OSR":"1","SNDR_nyq":"66.7","SFDR_nyq":"87.2","P_nyq":"1.30e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Delta-Sigma","sub_sub_class","DT Delta-Sigma","performance":{"source":"measured","tech":"180","fs":"5.8e6","OSR":"145","SNDR_nyq":"105.4","SFDR_nyq":"","P_nyq":"2.04e-4","DR":"108.8"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"130e6","OSR":"1","SNDR_nyq":"72.5","SFDR_nyq":"87.5","P_nyq":"820e-6"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"62.3","SFDR_nyq":"75.5","P_nyq":"3.3e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Delta-Sigma","sub_sub_class","DT Delta-Sigma","performance":{"source":"measured","tech":"28","fs":"950e6","OSR":"10","SNDR_nyq":"67","SFDR_nyq":"","P_nyq":"4.7e-3","DR":"70"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"100e6","OSR":"1","SNDR_nyq":"71.7","SFDR_nyq":"85.1","P_nyq":"0.7e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Oversampling","sub_sub_class","NS-SAR","performance":{"source":"measured","tech":"40","fs":"10e6","OSR":"8","SNDR_nyq":"83.8","SFDR_nyq":"","P_nyq":"107e-6","DR":"85.5"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"100e6","OSR":"1","SNDR_nyq":"72.6","SFDR_nyq":"86.5","P_nyq":"2.5e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"600e6","OSR":"1","SNDR_nyq":"58.7","SFDR_nyq":"72.4","P_nyq":"14.5e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"1e9","OSR":"1","SNDR_nyq":"56.6","SFDR_nyq":"73.1","P_nyq":"24.8e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"180","fs":"15e6","OSR":"1","SNDR_nyq":"88.0","SFDR_nyq":"96.5","P_nyq":"9.8e-3", "DR":"93.9"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"90","fs":"24e6","OSR":"1","SNDR_nyq":"74.3","SFDR_nyq":"85.5","P_nyq":"5.1e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"600e6","OSR":"1","SNDR_nyq":"60.2","SFDR_nyq":"78.3","P_nyq":"6.0e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"3.2e9","OSR":"1","SNDR_nyq":"61.7","SFDR_nyq":"73.3","P_nyq":"61.3e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"600e6","OSR":"1","SNDR_nyq":"56.3","SFDR_nyq":"69.2","P_nyq":"14.2e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"100e6","OSR":"1","SNDR_nyq":"90.4","SFDR_nyq":"90.4","P_nyq":"2.3e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"72.32","SFDR_nyq":"78.13","P_nyq":"2.74e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"65","fs":"100e6","OSR":"1","SNDR_nyq":"56.6","SFDR_nyq":"64.7","P_nyq":"2.46e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Pipelined-SAR","performance":{"source":"measured","tech":"65","fs":"50e6","OSR":"1","SNDR_nyq":"70.9","SFDR_nyq":"84.6","P_nyq":"1.0e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"65","fs":"100e6","OSR":"1","SNDR_nyq":"56.3","SFDR_nyq":"67.6","P_nyq":"2.46e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"75.9","SFDR_nyq":"91.4","P_nyq":"2.96e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"30e6","OSR":"1","SNDR_nyq":"61.5","SFDR_nyq":"74.2","P_nyq":"2.6e-3"}}</t>
-  </si>
-  <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class","Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"76.8","SFDR_nyq":"95.4","P_nyq":"5.1e-3"}}</t>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"76.8","SFDR_nyq":"95.4","P_nyq":"5.1e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"30e6","OSR":"1","SNDR_nyq":"61.5","SFDR_nyq":"74.2","P_nyq":"2.6e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"75.9","SFDR_nyq":"91.4","P_nyq":"2.96e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"65","fs":"100e6","OSR":"1","SNDR_nyq":"56.3","SFDR_nyq":"67.6","P_nyq":"2.46e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"65","fs":"50e6","OSR":"1","SNDR_nyq":"70.9","SFDR_nyq":"84.6","P_nyq":"1.0e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"65","fs":"100e6","OSR":"1","SNDR_nyq":"56.6","SFDR_nyq":"64.7","P_nyq":"2.46e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"72.32","SFDR_nyq":"78.13","P_nyq":"2.74e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"100e6","OSR":"1","SNDR_nyq":"90.4","SFDR_nyq":"90.4","P_nyq":"2.3e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"600e6","OSR":"1","SNDR_nyq":"56.3","SFDR_nyq":"69.2","P_nyq":"14.2e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"180","fs":"15e6","OSR":"1","SNDR_nyq":"88.0","SFDR_nyq":"96.5","P_nyq":"9.8e-3", "DR":"93.9"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"3.2e9","OSR":"1","SNDR_nyq":"61.7","SFDR_nyq":"73.3","P_nyq":"61.3e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"600e6","OSR":"1","SNDR_nyq":"60.2","SFDR_nyq":"78.3","P_nyq":"6.0e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"1e9","OSR":"1","SNDR_nyq":"56.6","SFDR_nyq":"73.1","P_nyq":"24.8e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"90","fs":"24e6","OSR":"1","SNDR_nyq":"74.3","SFDR_nyq":"85.5","P_nyq":"5.1e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"600e6","OSR":"1","SNDR_nyq":"58.7","SFDR_nyq":"72.4","P_nyq":"14.5e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"100e6","OSR":"1","SNDR_nyq":"72.6","SFDR_nyq":"86.5","P_nyq":"2.5e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Oversampling","sub_sub_class":"NS-SAR","performance":{"source":"measured","tech":"40","fs":"10e6","OSR":"8","SNDR_nyq":"83.8","SFDR_nyq":"","P_nyq":"107e-6","DR":"85.5"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"100e6","OSR":"1","SNDR_nyq":"71.7","SFDR_nyq":"85.1","P_nyq":"0.7e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"SAR","sub_sub_class":"NS-SAR","performance":{"source":"measured","tech":"40","fs":"10e6","OSR":"8","SNDR_nyq":"83.8","SFDR_nyq":"94.3","P_nyq":"107e-6"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"100e6","OSR":"1","SNDR_nyq":"71.7","SFDR_nyq":"87.2","P_nyq":"0.7e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"1e9","OSR":"1","SNDR_nyq":"59.5","SFDR_nyq":"75.9","P_nyq":"10.9e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"40e6","OSR":"1","SNDR_nyq":"75.7","SFDR_nyq":"81.4","P_nyq":"8.21e-4"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"4e9","OSR":"1","SNDR_nyq":"61.9","SFDR_nyq":"75.2","P_nyq":"75e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"75.5","SFDR_nyq":"62.3","P_nyq":"2.8e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"200e6","OSR":"1","SNDR_nyq":"66.7","SFDR_nyq":"87.2","P_nyq":"1.30e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Delta-Sigma","sub_sub_class":"DT Delta-Sigma","performance":{"source":"measured","tech":"180","fs":"5.8e6","OSR":"145","SNDR_nyq":"105.4","SFDR_nyq":"","P_nyq":"2.04e-4","DR":"108.8"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"130e6","OSR":"1","SNDR_nyq":"72.5","SFDR_nyq":"87.5","P_nyq":"820e-6"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"62.3","SFDR_nyq":"75.5","P_nyq":"3.3e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Delta-Sigma","sub_sub_class":"DT Delta-Sigma","performance":{"source":"measured","tech":"28","fs":"950e6","OSR":"10","SNDR_nyq":"67","SFDR_nyq":"","P_nyq":"4.7e-3","DR":"70"}}</t>
   </si>
 </sst>
 </file>
@@ -4743,8 +4743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4811,7 +4811,7 @@
         <v>179</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4838,7 +4838,7 @@
         <v>106</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4865,7 +4865,7 @@
         <v>171</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>409</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4892,7 +4892,7 @@
         <v>102</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4919,7 +4919,7 @@
         <v>218</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>407</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -4971,7 +4971,7 @@
         <v>160</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4998,7 +4998,7 @@
         <v>258</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5025,7 +5025,7 @@
         <v>255</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -5152,7 +5152,7 @@
         <v>164</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -5306,7 +5306,7 @@
         <v>226</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5333,7 +5333,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -5738,7 +5738,7 @@
         <v>131</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5767,7 +5767,7 @@
         <v>68</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5794,7 +5794,7 @@
         <v>73</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5821,7 +5821,7 @@
         <v>292</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5848,7 +5848,7 @@
         <v>77</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5875,7 +5875,7 @@
         <v>280</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5981,7 +5981,7 @@
         <v>121</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -6084,7 +6084,7 @@
         <v>314</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6111,7 +6111,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>393</v>
+        <v>399</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -6167,7 +6167,7 @@
         <v>309</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6194,7 +6194,7 @@
         <v>336</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -6271,7 +6271,7 @@
         <v>60</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -6427,7 +6427,7 @@
         <v>304</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6454,7 +6454,7 @@
         <v>51</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6483,7 +6483,7 @@
         <v>13</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -6637,7 +6637,7 @@
         <v>40</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6664,7 +6664,7 @@
         <v>343</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6691,7 +6691,7 @@
         <v>109</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6718,7 +6718,7 @@
         <v>24</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6745,7 +6745,7 @@
         <v>21</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>391</v>
+        <v>409</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -6876,7 +6876,7 @@
         <v>358</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -6977,7 +6977,7 @@
         <v>376</v>
       </c>
       <c r="I85" s="5" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update figure formatting and some spreadsheet aspects
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bhershbe\github\RingampSurvey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1329" documentId="8_{DF39C3F4-3D1F-4401-A869-CC4FEA15FC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC67EF8E-8A76-4D89-9E23-4D45A8563597}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4324925C-13B0-4F54-9512-B4D26668156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="27770" windowHeight="17640" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="27770" windowHeight="17640" activeTab="1" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="410">
   <si>
     <t>Title</t>
   </si>
@@ -1053,9 +1053,6 @@
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>(2022 still incomplete)</t>
   </si>
   <si>
     <t>a quick sanity check here…</t>
@@ -4743,8 +4740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4784,7 +4781,7 @@
         <v>1</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4811,7 +4808,7 @@
         <v>179</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4838,7 +4835,7 @@
         <v>106</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4865,7 +4862,7 @@
         <v>171</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4892,7 +4889,7 @@
         <v>102</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4919,7 +4916,7 @@
         <v>218</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -4971,7 +4968,7 @@
         <v>160</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4998,7 +4995,7 @@
         <v>258</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5025,7 +5022,7 @@
         <v>255</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -5152,7 +5149,7 @@
         <v>164</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -5306,7 +5303,7 @@
         <v>226</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5333,7 +5330,7 @@
         <v>98</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -5738,7 +5735,7 @@
         <v>131</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5767,7 +5764,7 @@
         <v>68</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5794,7 +5791,7 @@
         <v>73</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5821,7 +5818,7 @@
         <v>292</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5848,7 +5845,7 @@
         <v>77</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5875,7 +5872,7 @@
         <v>280</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5902,7 +5899,7 @@
         <v>11</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -5981,7 +5978,7 @@
         <v>121</v>
       </c>
       <c r="I47" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -6069,7 +6066,7 @@
         <v>311</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>312</v>
@@ -6084,7 +6081,7 @@
         <v>314</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6111,7 +6108,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -6152,7 +6149,7 @@
         <v>311</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>307</v>
@@ -6167,7 +6164,7 @@
         <v>309</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6194,7 +6191,7 @@
         <v>336</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -6271,7 +6268,7 @@
         <v>60</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -6310,7 +6307,7 @@
         <v>134</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>316</v>
@@ -6369,7 +6366,7 @@
         <v>33</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>34</v>
@@ -6427,7 +6424,7 @@
         <v>304</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6454,7 +6451,7 @@
         <v>51</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6483,7 +6480,7 @@
         <v>13</v>
       </c>
       <c r="I66" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -6572,7 +6569,7 @@
         <v>330</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>321</v>
@@ -6637,7 +6634,7 @@
         <v>40</v>
       </c>
       <c r="I72" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6652,19 +6649,19 @@
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="G73" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="H73" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="G73" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>343</v>
-      </c>
       <c r="I73" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6691,7 +6688,7 @@
         <v>109</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="75" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6718,7 +6715,7 @@
         <v>24</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6745,7 +6742,7 @@
         <v>21</v>
       </c>
       <c r="I76" s="13" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -6787,16 +6784,16 @@
         <v>327</v>
       </c>
       <c r="E78" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="F78" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="F78" s="6" t="s">
+      <c r="G78" s="7" t="s">
         <v>346</v>
       </c>
-      <c r="G78" s="7" t="s">
+      <c r="H78" s="7" t="s">
         <v>347</v>
-      </c>
-      <c r="H78" s="7" t="s">
-        <v>348</v>
       </c>
       <c r="I78" s="5"/>
     </row>
@@ -6812,16 +6809,16 @@
       </c>
       <c r="D79" s="6"/>
       <c r="E79" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I79" s="5"/>
     </row>
@@ -6833,22 +6830,22 @@
         <v>86</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>224</v>
       </c>
       <c r="E80" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="F80" s="8" t="s">
         <v>351</v>
       </c>
-      <c r="F80" s="8" t="s">
+      <c r="G80" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="H80" s="7" t="s">
         <v>352</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>353</v>
       </c>
       <c r="I80" s="5"/>
     </row>
@@ -6864,19 +6861,19 @@
       </c>
       <c r="D81" s="6"/>
       <c r="E81" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F81" s="7" t="s">
         <v>22</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H81" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I81" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -6884,23 +6881,23 @@
         <v>2022</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>229</v>
       </c>
       <c r="D82" s="6"/>
       <c r="E82" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="G82" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="H82" s="7" t="s">
         <v>360</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>361</v>
       </c>
       <c r="I82" s="5"/>
     </row>
@@ -6912,20 +6909,20 @@
         <v>12</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D83" s="6"/>
       <c r="E83" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="F83" s="7" t="s">
         <v>365</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="G83" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="G83" s="7" t="s">
+      <c r="H83" s="7" t="s">
         <v>367</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>368</v>
       </c>
       <c r="I83" s="5"/>
     </row>
@@ -6941,16 +6938,16 @@
       </c>
       <c r="D84" s="6"/>
       <c r="E84" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="F84" s="8" t="s">
+      <c r="G84" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="H84" s="8" t="s">
         <v>372</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -6965,19 +6962,19 @@
       </c>
       <c r="D85" s="6"/>
       <c r="E85" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>376</v>
+      </c>
+      <c r="H85" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>376</v>
-      </c>
       <c r="I85" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -7025,9 +7022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F627AA-E3AE-4351-92AE-68BECE4A1E4C}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7142,11 +7137,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>339</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>331</v>
@@ -7247,7 +7237,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B28" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$D$997,Analysis!A28)</f>
@@ -7265,7 +7255,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
moving some files around
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bhershbe\github\RingampSurvey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4324925C-13B0-4F54-9512-B4D26668156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A854F-77B8-4C43-BFEF-0A288797FA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="27770" windowHeight="17640" activeTab="1" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="27770" windowHeight="17640" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="411">
   <si>
     <t>Title</t>
   </si>
@@ -1278,6 +1278,9 @@
   </si>
   <si>
     <t>{"class":"ADC","sub_class”":"Delta-Sigma","sub_sub_class":"DT Delta-Sigma","performance":{"source":"measured","tech":"28","fs":"950e6","OSR":"10","SNDR_nyq":"67","SFDR_nyq":"","P_nyq":"4.7e-3","DR":"70"}}</t>
+  </si>
+  <si>
+    <t>(2022 still incomplete)</t>
   </si>
 </sst>
 </file>
@@ -4740,9 +4743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7022,7 +7023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F627AA-E3AE-4351-92AE-68BECE4A1E4C}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -7137,6 +7140,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>410</v>
+      </c>
+    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>331</v>

</xml_diff>

<commit_message>
fixed some typos in the json data
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\bhershbe\github\RingampSurvey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\benjamin\github\RingampSurvey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381A854F-77B8-4C43-BFEF-0A288797FA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE409D0-DD55-46B3-9E1B-D4568F5B5135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="27770" windowHeight="17640" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="8670" yWindow="3440" windowWidth="28800" windowHeight="15450" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
@@ -1214,9 +1214,6 @@
     <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"180","fs":"20e6","OSR":"1","SNDR_nyq":"72.32","SFDR_nyq":"78.13","P_nyq":"2.74e-3"}}</t>
   </si>
   <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"100e6","OSR":"1","SNDR_nyq":"90.4","SFDR_nyq":"90.4","P_nyq":"2.3e-3"}}</t>
-  </si>
-  <si>
     <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"28","fs":"600e6","OSR":"1","SNDR_nyq":"56.3","SFDR_nyq":"69.2","P_nyq":"14.2e-3"}}</t>
   </si>
   <si>
@@ -1262,9 +1259,6 @@
     <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Deep-Pipeline","performance":{"source":"measured","tech":"16","fs":"4e9","OSR":"1","SNDR_nyq":"61.9","SFDR_nyq":"75.2","P_nyq":"75e-3"}}</t>
   </si>
   <si>
-    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"75.5","SFDR_nyq":"62.3","P_nyq":"2.8e-3"}}</t>
-  </si>
-  <si>
     <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"28","fs":"200e6","OSR":"1","SNDR_nyq":"66.7","SFDR_nyq":"87.2","P_nyq":"1.30e-3"}}</t>
   </si>
   <si>
@@ -1281,6 +1275,12 @@
   </si>
   <si>
     <t>(2022 still incomplete)</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"40","fs":"100e6","OSR":"1","SNDR_nyq":"73.2","SFDR_nyq":"90.4","P_nyq":"2.3e-3"}}</t>
+  </si>
+  <si>
+    <t>{"class":"ADC","sub_class”":"Pipelined","sub_sub_class":"Pipelined-SAR","performance":{"source":"measured","tech":"16","fs":"500e6","OSR":"1","SNDR_nyq":"62.9","SFDR_nyq":"75.5","P_nyq":"2.8e-3"}}</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1367,31 +1367,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4741,9 +4728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I73" sqref="I73"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4781,2232 +4770,2119 @@
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="A2" s="3">
         <v>2012</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="8" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>2012</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <v>2012</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
+      <c r="A5" s="3">
         <v>2013</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <v>2014</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <v>2015</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <v>2015</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="3" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>2015</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="3" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <v>2015</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="3" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>2016</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <v>2016</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
+      <c r="A13" s="3">
         <v>2016</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>2016</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+      <c r="A15" s="3">
         <v>2017</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="3" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+      <c r="A16" s="3">
         <v>2017</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="A17" s="3">
         <v>2017</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+      <c r="A18" s="3">
         <v>2017</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+      <c r="A19" s="3">
         <v>2017</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+      <c r="A20" s="3">
         <v>2017</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6" t="s">
+      <c r="E20" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="A21" s="3">
         <v>2017</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6">
-        <v>2017</v>
-      </c>
-      <c r="B22" s="6" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>2018</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>2019</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>2020</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C58" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="D58" s="3"/>
+      <c r="E58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="D64" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B25" s="6" t="s">
+      <c r="E67" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="I67"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I68"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I69"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I70"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="I71"/>
+    </row>
+    <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="3">
+        <v>2021</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I76" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C78" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G78" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B26" s="6" t="s">
+      <c r="D81" s="3"/>
+      <c r="E81" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="H81" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G83" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A84" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C84" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="H84" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="3">
+        <v>2022</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="I26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="6">
-        <v>2018</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A33" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A34" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A36" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="I43" s="5" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="6">
-        <v>2019</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A49" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H52" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="I53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>335</v>
-      </c>
-      <c r="G55" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="I56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="6">
-        <v>2020</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H58" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="H59" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>319</v>
-      </c>
-      <c r="H60" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C61" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H61" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G65" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H65" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="13" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A67" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="I67" s="13"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A68" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I68" s="13"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C69" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="I69" s="13"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="I70" s="13"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A71" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="I71" s="13"/>
-    </row>
-    <row r="72" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="6">
-        <v>2021</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I72" s="11" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="F73" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="I73" s="11" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I74" s="11" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H75" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I75" s="11" t="s">
+      <c r="D85" s="3"/>
+      <c r="E85" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="G85" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H76" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I76" s="13" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A77" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="H77" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A78" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>327</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="H78" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A79" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>353</v>
-      </c>
-      <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A80" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>351</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D81" s="6"/>
-      <c r="E81" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="H81" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A82" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D82" s="6"/>
-      <c r="E82" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="F82" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="H82" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A83" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="D83" s="6"/>
-      <c r="E83" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="F83" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D84" s="6"/>
-      <c r="E84" s="8" t="s">
-        <v>370</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="G84" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="H84" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="6">
-        <v>2022</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="H85" s="8" t="s">
-        <v>375</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
-      <c r="C86" s="9"/>
-      <c r="D86" s="9"/>
-      <c r="E86" s="9"/>
-      <c r="F86" s="9"/>
-      <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A88" s="9"/>
-      <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H77">
@@ -7142,7 +7018,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Moved "interesting counter arguments" to a separate file
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14EF71A4-3757-42F0-A662-75076A0F1786}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E613743B-70C7-457E-8B14-69337C47C47D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
-    <sheet name="Interesting Counter-Arguments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="600">
   <si>
     <t>Title</t>
   </si>
@@ -1570,18 +1569,6 @@
   </si>
   <si>
     <t>10.1109/ASID60355.2023.10426347</t>
-  </si>
-  <si>
-    <t>Hsieh, Sung-En and Wu, Tzu-Chien and Hou, Chun-Chih</t>
-  </si>
-  <si>
-    <t>Good FoM with simple OTA</t>
-  </si>
-  <si>
-    <t>A 1.8GHz 12b Pre-Sampling Pipelined ADC with Reference Buffer and OP Power Relaxations</t>
-  </si>
-  <si>
-    <t>10.1109/ISSCC42615.2023.10067258</t>
   </si>
   <si>
     <t>Hu, Hang and Vesely, Vladimir and Moon, Un-Ku</t>
@@ -1855,7 +1842,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1879,12 +1866,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1894,7 +1875,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1902,35 +1883,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFDDDDDD"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFDDDDDD"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFDDDDDD"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDDDDDD"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1940,12 +1897,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2952,37 +2903,43 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$A$37:$A$46</c:f>
+              <c:f>Analysis!$A$38:$A$49</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>JSSC</c:v>
+                  <c:v>ISSCC</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>ISSCC</c:v>
+                  <c:v>VLSI</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>VLSI</c:v>
+                  <c:v>CICC</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CICC</c:v>
+                  <c:v>ESSERC</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>ESSCIRC</c:v>
+                  <c:v>ASSCC</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>ASSCC</c:v>
+                  <c:v>RFIC</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>ISCAS</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>JSSC</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>TCAS-I</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>TCAS-II</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
+                  <c:v>TVLSI</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Other</c:v>
                 </c:pt>
               </c:strCache>
@@ -2990,39 +2947,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$B$37:$B$46</c:f>
+              <c:f>Analysis!$B$38:$B$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>37</c:v>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5309,8 +5272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
   <dimension ref="A1:I132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
@@ -5506,7 +5469,7 @@
         <v>118</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -5610,7 +5573,7 @@
         <v>188</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -5636,7 +5599,7 @@
         <v>114</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -5647,7 +5610,7 @@
         <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>209</v>
@@ -5662,7 +5625,7 @@
         <v>211</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -5688,7 +5651,7 @@
         <v>141</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -5725,7 +5688,7 @@
         <v>128</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>124</v>
@@ -5740,7 +5703,7 @@
         <v>127</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -5769,7 +5732,7 @@
         <v>207</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -5795,7 +5758,7 @@
         <v>93</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -5821,7 +5784,7 @@
         <v>156</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -5832,7 +5795,7 @@
         <v>145</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>142</v>
@@ -5847,7 +5810,7 @@
         <v>146</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -5925,7 +5888,7 @@
         <v>80</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -5936,7 +5899,7 @@
         <v>190</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>191</v>
@@ -5951,7 +5914,7 @@
         <v>192</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -5980,7 +5943,7 @@
         <v>89</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -6006,7 +5969,7 @@
         <v>214</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -6032,7 +5995,7 @@
         <v>84</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -6043,7 +6006,7 @@
         <v>86</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>286</v>
@@ -6058,7 +6021,7 @@
         <v>288</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -6069,7 +6032,7 @@
         <v>86</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>246</v>
@@ -6084,7 +6047,7 @@
         <v>248</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -6110,7 +6073,7 @@
         <v>151</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -6121,7 +6084,7 @@
         <v>239</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>236</v>
@@ -6136,7 +6099,7 @@
         <v>238</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -6165,7 +6128,7 @@
         <v>276</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -6176,7 +6139,7 @@
         <v>136</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>133</v>
@@ -6191,7 +6154,7 @@
         <v>137</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -6217,7 +6180,7 @@
         <v>272</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -6243,7 +6206,7 @@
         <v>63</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -6269,7 +6232,7 @@
         <v>175</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -6280,7 +6243,7 @@
         <v>86</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>166</v>
@@ -6295,7 +6258,7 @@
         <v>168</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -6515,7 +6478,7 @@
         <v>222</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -6541,7 +6504,7 @@
         <v>296</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -6567,7 +6530,7 @@
         <v>123</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -6593,7 +6556,7 @@
         <v>184</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -6619,7 +6582,7 @@
         <v>55</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -6645,7 +6608,7 @@
         <v>231</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -6729,7 +6692,7 @@
         <v>244</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -6810,7 +6773,7 @@
         <v>235</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -6821,7 +6784,7 @@
         <v>239</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>282</v>
@@ -6836,7 +6799,7 @@
         <v>284</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
@@ -6888,7 +6851,7 @@
         <v>264</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -6899,7 +6862,7 @@
         <v>319</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>305</v>
@@ -6917,7 +6880,7 @@
         <v>318</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -6943,7 +6906,7 @@
         <v>31</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -6966,10 +6929,10 @@
         <v>33</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -6995,7 +6958,7 @@
         <v>199</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -7090,7 +7053,7 @@
         <v>145</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>201</v>
@@ -7105,7 +7068,7 @@
         <v>203</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -7131,7 +7094,7 @@
         <v>44</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -7157,7 +7120,7 @@
         <v>252</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -7186,7 +7149,7 @@
         <v>323</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -7197,7 +7160,7 @@
         <v>239</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>265</v>
@@ -7212,7 +7175,7 @@
         <v>268</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -7249,22 +7212,22 @@
         <v>128</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -7293,7 +7256,7 @@
         <v>345</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -7322,7 +7285,7 @@
         <v>375</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -7348,7 +7311,7 @@
         <v>367</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -7368,13 +7331,13 @@
         <v>370</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -7515,7 +7478,7 @@
         <v>12</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E83" s="3" t="s">
         <v>363</v>
@@ -7530,7 +7493,7 @@
         <v>365</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -7556,7 +7519,7 @@
         <v>374</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -7582,7 +7545,7 @@
         <v>353</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -7608,7 +7571,7 @@
         <v>300</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -7622,7 +7585,7 @@
         <v>65</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>298</v>
@@ -7637,7 +7600,7 @@
         <v>300</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -7663,7 +7626,7 @@
         <v>361</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -7689,7 +7652,7 @@
         <v>361</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -7700,7 +7663,7 @@
         <v>506</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>507</v>
@@ -7718,7 +7681,7 @@
         <v>509</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -7732,19 +7695,19 @@
         <v>65</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I91" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -7773,7 +7736,7 @@
         <v>406</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -7787,19 +7750,19 @@
         <v>65</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="G93" s="3" t="s">
         <v>434</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -7825,7 +7788,7 @@
         <v>413</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -7833,25 +7796,25 @@
         <v>2023</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="H95" s="3" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -7859,25 +7822,25 @@
         <v>2023</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -7903,7 +7866,7 @@
         <v>474</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -7929,7 +7892,7 @@
         <v>478</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -7955,7 +7918,7 @@
         <v>478</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
@@ -7984,7 +7947,7 @@
         <v>499</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -7992,25 +7955,25 @@
         <v>2023</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="H101" s="3" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
@@ -8036,7 +7999,7 @@
         <v>469</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -8065,7 +8028,7 @@
         <v>495</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
@@ -8076,7 +8039,7 @@
         <v>462</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>458</v>
@@ -8091,7 +8054,7 @@
         <v>460</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
@@ -8117,7 +8080,7 @@
         <v>416</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
@@ -8128,22 +8091,22 @@
         <v>418</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="H106" s="3" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="I106" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
@@ -8172,7 +8135,7 @@
         <v>465</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
@@ -8180,28 +8143,28 @@
         <v>2024</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I108" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -8209,7 +8172,7 @@
         <v>2024</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>65</v>
@@ -8227,7 +8190,7 @@
         <v>446</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
@@ -8235,25 +8198,25 @@
         <v>2024</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
@@ -8261,28 +8224,28 @@
         <v>2024</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="H111" s="3" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
@@ -8311,7 +8274,7 @@
         <v>451</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.35">
@@ -8334,7 +8297,7 @@
         <v>426</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.35">
@@ -8363,7 +8326,7 @@
         <v>486</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.35">
@@ -8377,19 +8340,19 @@
         <v>65</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.35">
@@ -8397,25 +8360,25 @@
         <v>2024</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="H116" s="3" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.35">
@@ -8444,7 +8407,7 @@
         <v>420</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.35">
@@ -8470,7 +8433,7 @@
         <v>424</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.35">
@@ -8496,7 +8459,7 @@
         <v>432</v>
       </c>
       <c r="I119" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.35">
@@ -8522,7 +8485,7 @@
         <v>435</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.35">
@@ -8551,7 +8514,7 @@
         <v>481</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.35">
@@ -8562,7 +8525,7 @@
         <v>12</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>502</v>
@@ -8577,7 +8540,7 @@
         <v>503</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.35">
@@ -8591,19 +8554,19 @@
         <v>65</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="I123" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.35">
@@ -8632,7 +8595,7 @@
         <v>457</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.35">
@@ -8640,25 +8603,25 @@
         <v>2024</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H125" s="3" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="I125" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.35">
@@ -8672,19 +8635,19 @@
         <v>65</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="H126" s="3" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.35">
@@ -8698,19 +8661,19 @@
         <v>65</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.35">
@@ -8724,19 +8687,19 @@
         <v>36</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="H128" s="3" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.35">
@@ -8762,7 +8725,7 @@
         <v>489</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.35">
@@ -8788,7 +8751,7 @@
         <v>439</v>
       </c>
       <c r="I130" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.35">
@@ -8814,7 +8777,7 @@
         <v>443</v>
       </c>
       <c r="I131" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.35">
@@ -8822,25 +8785,25 @@
         <v>2024</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
   </sheetData>
@@ -8855,10 +8818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F627AA-E3AE-4351-92AE-68BECE4A1E4C}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M49" sqref="M49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9092,7 +9055,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B28" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$D$997,Analysis!A28)</f>
@@ -9101,7 +9064,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B29" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$D$997,Analysis!A29)</f>
@@ -9139,15 +9102,6 @@
         <v>328</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="3">
-        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A37)</f>
-        <v>24</v>
-      </c>
-    </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>8</v>
@@ -9177,11 +9131,11 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>594</v>
       </c>
       <c r="B41" s="3">
-        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A41)</f>
-        <v>3</v>
+        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,"ESSCIRC")+COUNTIF('Ringamp Publication List'!$B$2:$B$997,"ESSERC")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -9195,116 +9149,69 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>530</v>
       </c>
       <c r="B43" s="3">
         <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A43)</f>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="B44" s="3">
         <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A44)</f>
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>239</v>
+        <v>12</v>
       </c>
       <c r="B45" s="3">
         <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A45)</f>
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="3">
+        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A46)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" s="3">
+        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A47)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>418</v>
+      </c>
+      <c r="B48" s="3">
+        <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A48)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>337</v>
       </c>
-      <c r="B46" s="3">
-        <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)-SUM(B37:B45)</f>
-        <v>37</v>
+      <c r="B49" s="3">
+        <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)-SUM(B38:B48)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767B74E5-BA40-4035-838C-6038FA255288}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="8.7265625" style="3"/>
-    <col min="3" max="3" width="20.54296875" style="3" customWidth="1"/>
-    <col min="4" max="8" width="25" style="3" customWidth="1"/>
-    <col min="9" max="9" width="25.453125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
-        <v>2023</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>512</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>514</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added 2 new papers
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83318DCB-DEDF-41E9-AE4D-F84F867709C8}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B4E36E-F743-4620-92FD-93A3AA5FEC56}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="610">
   <si>
     <t>Title</t>
   </si>
@@ -1839,6 +1839,33 @@
   </si>
   <si>
     <t>All other</t>
+  </si>
+  <si>
+    <t>12b 500MS/s successive-approximation-registerassisted pipeline analogue-to-digital convertor using a four-stage ring amplifier with coarse-analogue-to-digital convertor embedded</t>
+  </si>
+  <si>
+    <t>10.1049/ell2.70101</t>
+  </si>
+  <si>
+    <t>Liu, Linghao &amp; Ren, Junyan &amp; Fan, Ye.</t>
+  </si>
+  <si>
+    <t>E. Letters</t>
+  </si>
+  <si>
+    <t>This article presents a 12b 500MS/s successive‐approximation‐register‐assisted pipeline analogue‐to‐digital converter. By adopting a new auto‐zero scheme, a calibration‐free four‐stage ring residue amplifier with a small offset cancellation capacitor is proposed. In addition, the coarse‐analogue‐to‐digital converter of the second stage is embedded into the amplification phase, which relaxes the comparison periods of the first and second stages by 25.0% and 17.4%, respectively. Post‐simulated in 28‐nm CMOS technology with a 0.9 V supply, the analogue‐to‐digital converter achieves 62.2 dB SNDR and 78.1 dB SFDR. It consumes 8.45 mW with an on‐chip reference voltage buffer, resulting in Schreier's figure of merit (FoMS) of 166.9 dB.</t>
+  </si>
+  <si>
+    <t>Ye, Siyuan and Gao, Jihang and Li, Jie and Chen, Zhuoyi and Xu, Xinhang and Cui, Jiajia and Luan, Yaohui and Ye, Le and Zhang, Xing and Huang, Ru and Shen, Linxiao</t>
+  </si>
+  <si>
+    <t>This work presents a 2-mW 70.7-dB SNDR 200-MS/s pipelined-successive-approximation-register (SAR) analog-to-digital converter (ADC) with a continuous-time SAR-assisted detect-and-skip (CTDAS) and open-then-close correlated level shifting (OCCLS). In the first-stage SAR ADC, we propose using the continuous-time SAR (CTSAR) as the coarse SAR ADC in the detect-and-skip (DAS) scheme, thus parallelizing MSB conversion with ADC sampling. Furthermore, in the residue amplifier (RA), an OCCLS technique is proposed, which significantly speeds up the first correlated level shifting (CLS) phase by open-loop amplification and consequently enhances the equivalent open-loop gain at negligible extra time cost. An on-chip background self-detect-and-cut loop is used for the OCCLS to attain a PVT-robust high equivalent open-loop gain. For RA implementation, a hybrid static–floating ring-amp structure is adopted to improve the noise performance while fitting in well with the OCCLS scheme. Thanks to the proposed techniques, the 22-nm prototype achieves 70.7-dB SNDR under 200 MS/s while consuming only 2.0 mW from a 0.9-V supply. It measures 177.7-dB FoMs, which is the highest among ADCs with equivalent or higher sampling rates.</t>
+  </si>
+  <si>
+    <t>10.1109/JSSC.2024.3497175</t>
+  </si>
+  <si>
+    <t>A 2-mW 70.7-dB SNDR 200-MS/s Pipelined-SAR ADC Using Continuous-Time SAR-Assisted Detect-and-Skip and Open-Then-Close Correlated Level Shifting</t>
   </si>
 </sst>
 </file>
@@ -2160,7 +2187,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2554,7 +2581,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13</c:v>
@@ -2993,7 +3020,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
@@ -3005,7 +3032,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5290,11 +5317,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6FCC8A-E42D-4F65-9CF1-EB965B6A3F77}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8827,6 +8854,128 @@
         <v>595</v>
       </c>
     </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A133" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E133" t="s">
+        <v>601</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H133" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="I133" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A134" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I135" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I136" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I137" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I138" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I139" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I140" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I141" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I142" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I143" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I144" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="145" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I145" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="146" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I146" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="147" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I147" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="148" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I148" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I132">
     <sortCondition ref="A2:A132"/>
@@ -8842,7 +8991,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8973,7 +9122,7 @@
       </c>
       <c r="B14" s="3">
         <f>COUNTIF('Ringamp Publication List'!$A$2:$A$995,Analysis!A14)</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -8999,7 +9148,7 @@
       </c>
       <c r="B19" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$D$997,Analysis!A19)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -9103,7 +9252,7 @@
       </c>
       <c r="B32" s="3">
         <f>SUM(B18:B29)</f>
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -9112,7 +9261,7 @@
       </c>
       <c r="B33" s="3">
         <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)</f>
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -9192,7 +9341,7 @@
       </c>
       <c r="B45" s="3">
         <f>COUNTIF('Ringamp Publication List'!$B$2:$B$997,Analysis!A45)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -9228,7 +9377,7 @@
       </c>
       <c r="B49" s="3">
         <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)-SUM(B38:B48)</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed initial state for spreadsheet when it opens
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -5320,8 +5320,8 @@
   <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added another 2024 paper, annotated Sim Only for certain papers
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B4E36E-F743-4620-92FD-93A3AA5FEC56}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBA6B347-6367-4606-BD49-3F6BE994F46F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
+    <workbookView xWindow="5980" yWindow="2950" windowWidth="28800" windowHeight="15370" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
   <sheets>
     <sheet name="Ringamp Publication List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="618">
   <si>
     <t>Title</t>
   </si>
@@ -1866,6 +1866,30 @@
   </si>
   <si>
     <t>A 2-mW 70.7-dB SNDR 200-MS/s Pipelined-SAR ADC Using Continuous-Time SAR-Assisted Detect-and-Skip and Open-Then-Close Correlated Level Shifting</t>
+  </si>
+  <si>
+    <t>A 12b 400MS/s 4-Time Interleaved Pipelined-SAR ADC with Fully Differential Bias-enhanced Ring Amplifier</t>
+  </si>
+  <si>
+    <t>Jian, Mingchao and Kong, Xiangjian and Zheng, Jiwei and Xie, Huanlin and Guo, Chunbing</t>
+  </si>
+  <si>
+    <t>10.1109/ICICM63644.2024.10814121</t>
+  </si>
+  <si>
+    <t>A 12-bit 400MS/s 4-channel time-interleaved pipelined-SAR ADC with a fully differential bias-enhanced ring amplifier for low-power and high-speed application is presented. The sub-ADC adopts a two-stage pipeline quantization scheme with a 6-bit SAR ADC in the first stage and a 7-bit SAR ADC in the second stage with 1-hit overlapping. To further optimize the speed of the sub-ADCs, a bias-enhanced ring amplifier is proposed. A prototype ADC is designed and simulated in 65nm CMOS technology with a standard 1.2 V supply voltage. With the least-mean-square algorithm calibration, this ADC achieves SNDR of 64.5 dB and SFDR of 86.6 dB. The whole ADC consumes 10.3mW, achieving a FoM of 19.9 fJ/conv-step.</t>
+  </si>
+  <si>
+    <t>ICICM</t>
+  </si>
+  <si>
+    <t>Interleaved, Sim only</t>
+  </si>
+  <si>
+    <t>Sim only</t>
+  </si>
+  <si>
+    <t>FIA, Sim only</t>
   </si>
 </sst>
 </file>
@@ -2187,7 +2211,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2581,7 +2605,7 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13</c:v>
@@ -2950,9 +2974,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Analysis!$A$38:$A$49</c:f>
+              <c:f>Analysis!$A$38:$A$48</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>ISSCC</c:v>
                 </c:pt>
@@ -2986,18 +3010,15 @@
                 <c:pt idx="10">
                   <c:v>TVLSI</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>All other</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Analysis!$B$38:$B$49</c:f>
+              <c:f>Analysis!$B$38:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -3030,9 +3051,6 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5320,7 +5338,7 @@
   <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -5504,6 +5522,9 @@
       <c r="C7" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>114</v>
       </c>
@@ -5608,6 +5629,9 @@
       <c r="C11" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>184</v>
       </c>
@@ -5660,6 +5684,9 @@
       <c r="C13" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>207</v>
       </c>
@@ -5819,6 +5846,9 @@
       <c r="C19" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E19" s="3" t="s">
         <v>151</v>
       </c>
@@ -5845,6 +5875,9 @@
       <c r="C20" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>140</v>
       </c>
@@ -5949,6 +5982,9 @@
       <c r="C24" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D24" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E24" s="3" t="s">
         <v>189</v>
       </c>
@@ -6004,6 +6040,9 @@
       <c r="C26" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E26" s="3" t="s">
         <v>211</v>
       </c>
@@ -6030,6 +6069,9 @@
       <c r="C27" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D27" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>81</v>
       </c>
@@ -6056,6 +6098,9 @@
       <c r="C28" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D28" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>284</v>
       </c>
@@ -6082,6 +6127,9 @@
       <c r="C29" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D29" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>244</v>
       </c>
@@ -6267,6 +6315,9 @@
       <c r="C36" s="3" t="s">
         <v>174</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E36" s="3" t="s">
         <v>171</v>
       </c>
@@ -6293,6 +6344,9 @@
       <c r="C37" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D37" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E37" s="3" t="s">
         <v>164</v>
       </c>
@@ -6941,6 +6995,9 @@
       <c r="C61" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D61" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E61" s="3" t="s">
         <v>28</v>
       </c>
@@ -6993,6 +7050,9 @@
       <c r="C63" s="3" t="s">
         <v>196</v>
       </c>
+      <c r="D63" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E63" s="3" t="s">
         <v>193</v>
       </c>
@@ -7580,6 +7640,9 @@
       <c r="C85" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="D85" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E85" s="3" t="s">
         <v>345</v>
       </c>
@@ -7849,6 +7912,9 @@
       <c r="C95" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D95" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E95" s="3" t="s">
         <v>542</v>
       </c>
@@ -8008,6 +8074,9 @@
       <c r="C101" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D101" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E101" s="3" t="s">
         <v>566</v>
       </c>
@@ -8413,6 +8482,9 @@
       <c r="C116" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D116" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E116" s="3" t="s">
         <v>529</v>
       </c>
@@ -8628,7 +8700,7 @@
         <v>64</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>303</v>
+        <v>617</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>451</v>
@@ -8838,6 +8910,9 @@
       <c r="C132" s="3" t="s">
         <v>596</v>
       </c>
+      <c r="D132" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E132" s="3" t="s">
         <v>561</v>
       </c>
@@ -8864,6 +8939,9 @@
       <c r="C133" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D133" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="E133" t="s">
         <v>601</v>
       </c>
@@ -8907,6 +8985,30 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A135" s="3">
+        <v>2024</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="H135" s="3" t="s">
+        <v>613</v>
+      </c>
       <c r="I135" s="3" t="s">
         <v>595</v>
       </c>
@@ -8991,7 +9093,7 @@
   <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9122,7 +9224,7 @@
       </c>
       <c r="B14" s="3">
         <f>COUNTIF('Ringamp Publication List'!$A$2:$A$995,Analysis!A14)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -9148,7 +9250,7 @@
       </c>
       <c r="B19" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$D$997,Analysis!A19)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -9252,7 +9354,7 @@
       </c>
       <c r="B32" s="3">
         <f>SUM(B18:B29)</f>
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -9261,7 +9363,7 @@
       </c>
       <c r="B33" s="3">
         <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)</f>
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -9377,7 +9479,7 @@
       </c>
       <c r="B49" s="3">
         <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)-SUM(B38:B48)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed category from "general" to "non-specific"
</commit_message>
<xml_diff>
--- a/data/RingampSurvey.xlsx
+++ b/data/RingampSurvey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/benjamin_hershberg_intel_com/Documents/Documents/GitHub/RingampSurvey/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23991DB4-EE27-4D68-90EC-226489D7B9E3}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="13_ncr:1_{9FBB236B-CF51-4197-B165-772080A6ED7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE0F2497-8378-4D60-93DF-358BBA7A2176}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="2140" windowWidth="23990" windowHeight="17770" xr2:uid="{F214066B-E69B-4EBB-B66C-26071D350487}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="621">
   <si>
     <t>Title</t>
   </si>
@@ -1815,9 +1815,6 @@
   </si>
   <si>
     <t>VCO, SAR, Interleaved</t>
-  </si>
-  <si>
-    <t>General</t>
   </si>
   <si>
     <t>This work presents a discrete-time (DT) delta sigma modulator (DSM) ADC that uses ring amplifiers to relax critical speed and efficiency bottlenecks. The DSM is designed as a 3 rd -order Cascade of Integrator with Feed Forward (CIFF) with a 4-bit quantizer, and it achieves a peak SNDR of 67dB and DR of 70.0dB with 47.5MHz bandwidth when clocked at 950MHz. This is the highest bandwidth reported to-date among single-channel DT DSM ADCs and demonstrates a viable alternative to continuous-time (CT) DSM ADCs for wideband oversampling applications. With a power consumption of 4.7mW from a 1V supply, FOMs and FOMw are 167.0dB and 27.0fJ/c.s. respectively, demonstrating efficient DT delta-sigma conversion with high bandwidth.</t>
@@ -2602,7 +2599,7 @@
                   <c:v>RF</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>General</c:v>
+                  <c:v>Non-Specific</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2647,7 +2644,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5350,8 +5347,8 @@
   <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5377,7 +5374,7 @@
         <v>325</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>93</v>
@@ -5409,7 +5406,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>175</v>
@@ -5438,7 +5435,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>102</v>
@@ -5467,7 +5464,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>167</v>
@@ -5496,7 +5493,7 @@
         <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>98</v>
@@ -5525,7 +5522,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>214</v>
@@ -5554,7 +5551,7 @@
         <v>327</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>114</v>
@@ -5569,7 +5566,7 @@
         <v>116</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -5583,7 +5580,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>156</v>
@@ -5612,7 +5609,7 @@
         <v>64</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>254</v>
@@ -5641,7 +5638,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>251</v>
@@ -5670,7 +5667,7 @@
         <v>327</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>184</v>
@@ -5685,7 +5682,7 @@
         <v>186</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -5699,7 +5696,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>109</v>
@@ -5714,7 +5711,7 @@
         <v>112</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -5725,10 +5722,10 @@
         <v>84</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>207</v>
@@ -5743,7 +5740,7 @@
         <v>209</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -5757,7 +5754,7 @@
         <v>327</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>137</v>
@@ -5772,7 +5769,7 @@
         <v>139</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -5786,7 +5783,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>159</v>
@@ -5812,10 +5809,10 @@
         <v>126</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>122</v>
@@ -5830,7 +5827,7 @@
         <v>125</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -5844,7 +5841,7 @@
         <v>64</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>324</v>
@@ -5862,7 +5859,7 @@
         <v>205</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -5876,7 +5873,7 @@
         <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>90</v>
@@ -5891,7 +5888,7 @@
         <v>91</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
@@ -5905,7 +5902,7 @@
         <v>327</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>151</v>
@@ -5920,7 +5917,7 @@
         <v>154</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
@@ -5931,10 +5928,10 @@
         <v>143</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>140</v>
@@ -5949,7 +5946,7 @@
         <v>144</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
@@ -5963,7 +5960,7 @@
         <v>64</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>222</v>
@@ -5992,7 +5989,7 @@
         <v>35</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>94</v>
@@ -6021,7 +6018,7 @@
         <v>35</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>76</v>
@@ -6036,7 +6033,7 @@
         <v>78</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
@@ -6047,10 +6044,10 @@
         <v>188</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>189</v>
@@ -6065,7 +6062,7 @@
         <v>190</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
@@ -6079,7 +6076,7 @@
         <v>64</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>324</v>
@@ -6097,7 +6094,7 @@
         <v>87</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
@@ -6111,7 +6108,7 @@
         <v>327</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>211</v>
@@ -6126,7 +6123,7 @@
         <v>212</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -6140,7 +6137,7 @@
         <v>35</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>81</v>
@@ -6155,7 +6152,7 @@
         <v>82</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -6166,10 +6163,10 @@
         <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>284</v>
@@ -6184,7 +6181,7 @@
         <v>286</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -6195,10 +6192,10 @@
         <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>244</v>
@@ -6213,7 +6210,7 @@
         <v>246</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -6227,7 +6224,7 @@
         <v>327</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>146</v>
@@ -6242,7 +6239,7 @@
         <v>149</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -6253,10 +6250,10 @@
         <v>237</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>234</v>
@@ -6271,7 +6268,7 @@
         <v>236</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -6285,7 +6282,7 @@
         <v>64</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>324</v>
@@ -6303,7 +6300,7 @@
         <v>274</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -6314,10 +6311,10 @@
         <v>134</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>131</v>
@@ -6332,7 +6329,7 @@
         <v>135</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -6346,7 +6343,7 @@
         <v>226</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>268</v>
@@ -6361,7 +6358,7 @@
         <v>270</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -6375,7 +6372,7 @@
         <v>64</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>61</v>
@@ -6390,7 +6387,7 @@
         <v>62</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -6404,7 +6401,7 @@
         <v>174</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>171</v>
@@ -6419,7 +6416,7 @@
         <v>173</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -6430,10 +6427,10 @@
         <v>84</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>164</v>
@@ -6448,7 +6445,7 @@
         <v>166</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -6462,7 +6459,7 @@
         <v>64</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>493</v>
@@ -6494,7 +6491,7 @@
         <v>35</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>324</v>
@@ -6509,7 +6506,7 @@
         <v>65</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>384</v>
@@ -6526,7 +6523,7 @@
         <v>35</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>70</v>
@@ -6555,7 +6552,7 @@
         <v>64</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>493</v>
@@ -6587,7 +6584,7 @@
         <v>35</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>73</v>
@@ -6616,7 +6613,7 @@
         <v>35</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>275</v>
@@ -6645,7 +6642,7 @@
         <v>35</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>9</v>
@@ -6674,7 +6671,7 @@
         <v>221</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>322</v>
@@ -6692,7 +6689,7 @@
         <v>220</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
@@ -6706,7 +6703,7 @@
         <v>64</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>291</v>
@@ -6721,7 +6718,7 @@
         <v>294</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -6735,7 +6732,7 @@
         <v>64</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>118</v>
@@ -6750,7 +6747,7 @@
         <v>121</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -6764,7 +6761,7 @@
         <v>35</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>180</v>
@@ -6779,7 +6776,7 @@
         <v>182</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
@@ -6793,7 +6790,7 @@
         <v>64</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>52</v>
@@ -6808,7 +6805,7 @@
         <v>54</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -6822,7 +6819,7 @@
         <v>226</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>225</v>
@@ -6837,7 +6834,7 @@
         <v>229</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
@@ -6851,7 +6848,7 @@
         <v>308</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>303</v>
@@ -6883,7 +6880,7 @@
         <v>64</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>3</v>
@@ -6912,7 +6909,7 @@
         <v>323</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>322</v>
@@ -6930,7 +6927,7 @@
         <v>242</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
@@ -6944,7 +6941,7 @@
         <v>308</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>303</v>
@@ -6976,7 +6973,7 @@
         <v>64</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>331</v>
@@ -7005,7 +7002,7 @@
         <v>327</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>230</v>
@@ -7020,7 +7017,7 @@
         <v>233</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -7031,10 +7028,10 @@
         <v>237</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>280</v>
@@ -7049,7 +7046,7 @@
         <v>282</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -7063,7 +7060,7 @@
         <v>35</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>57</v>
@@ -7092,7 +7089,7 @@
         <v>261</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>258</v>
@@ -7107,7 +7104,7 @@
         <v>262</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -7118,10 +7115,10 @@
         <v>317</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>303</v>
@@ -7139,7 +7136,7 @@
         <v>316</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -7153,7 +7150,7 @@
         <v>64</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>28</v>
@@ -7168,7 +7165,7 @@
         <v>30</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -7182,7 +7179,7 @@
         <v>327</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>34</v>
@@ -7194,10 +7191,10 @@
         <v>32</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
@@ -7211,7 +7208,7 @@
         <v>196</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>193</v>
@@ -7226,7 +7223,7 @@
         <v>197</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -7240,7 +7237,7 @@
         <v>35</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>303</v>
@@ -7272,7 +7269,7 @@
         <v>35</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>48</v>
@@ -7301,7 +7298,7 @@
         <v>35</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>324</v>
@@ -7316,7 +7313,7 @@
         <v>14</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="J66" s="3" t="s">
         <v>395</v>
@@ -7330,10 +7327,10 @@
         <v>143</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>199</v>
@@ -7348,7 +7345,7 @@
         <v>201</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
@@ -7362,7 +7359,7 @@
         <v>35</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>45</v>
@@ -7377,7 +7374,7 @@
         <v>43</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
@@ -7391,7 +7388,7 @@
         <v>327</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>247</v>
@@ -7406,7 +7403,7 @@
         <v>250</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
@@ -7420,7 +7417,7 @@
         <v>327</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>374</v>
@@ -7438,7 +7435,7 @@
         <v>321</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -7449,10 +7446,10 @@
         <v>237</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>263</v>
@@ -7467,7 +7464,7 @@
         <v>266</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
@@ -7481,7 +7478,7 @@
         <v>64</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>40</v>
@@ -7510,7 +7507,7 @@
         <v>555</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>552</v>
@@ -7525,7 +7522,7 @@
         <v>554</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
@@ -7539,7 +7536,7 @@
         <v>35</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>324</v>
@@ -7557,7 +7554,7 @@
         <v>342</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
@@ -7571,7 +7568,7 @@
         <v>352</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>221</v>
@@ -7589,7 +7586,7 @@
         <v>372</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
@@ -7603,7 +7600,7 @@
         <v>308</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>365</v>
@@ -7618,7 +7615,7 @@
         <v>364</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
@@ -7632,7 +7629,7 @@
         <v>308</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>365</v>
@@ -7647,7 +7644,7 @@
         <v>508</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
@@ -7661,7 +7658,7 @@
         <v>64</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>336</v>
@@ -7690,7 +7687,7 @@
         <v>327</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>106</v>
@@ -7719,7 +7716,7 @@
         <v>64</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>22</v>
@@ -7748,7 +7745,7 @@
         <v>64</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>19</v>
@@ -7777,7 +7774,7 @@
         <v>64</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>351</v>
@@ -7806,7 +7803,7 @@
         <v>527</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>360</v>
@@ -7821,7 +7818,7 @@
         <v>362</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
@@ -7835,7 +7832,7 @@
         <v>327</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>369</v>
@@ -7850,7 +7847,7 @@
         <v>371</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.35">
@@ -7864,7 +7861,7 @@
         <v>35</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>345</v>
@@ -7879,7 +7876,7 @@
         <v>350</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
@@ -7893,7 +7890,7 @@
         <v>64</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>296</v>
@@ -7908,7 +7905,7 @@
         <v>298</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
@@ -7922,7 +7919,7 @@
         <v>64</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>517</v>
@@ -7940,7 +7937,7 @@
         <v>298</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.35">
@@ -7954,7 +7951,7 @@
         <v>226</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>357</v>
@@ -7969,7 +7966,7 @@
         <v>358</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.35">
@@ -7983,7 +7980,7 @@
         <v>226</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>357</v>
@@ -7998,7 +7995,7 @@
         <v>358</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
@@ -8009,10 +8006,10 @@
         <v>502</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>503</v>
@@ -8030,7 +8027,7 @@
         <v>505</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
@@ -8044,7 +8041,7 @@
         <v>64</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>519</v>
@@ -8059,7 +8056,7 @@
         <v>520</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.35">
@@ -8073,7 +8070,7 @@
         <v>35</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>406</v>
@@ -8091,7 +8088,7 @@
         <v>403</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.35">
@@ -8105,7 +8102,7 @@
         <v>64</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>509</v>
@@ -8120,7 +8117,7 @@
         <v>511</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.35">
@@ -8134,7 +8131,7 @@
         <v>327</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>408</v>
@@ -8149,7 +8146,7 @@
         <v>410</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.35">
@@ -8160,10 +8157,10 @@
         <v>543</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>542</v>
@@ -8178,7 +8175,7 @@
         <v>544</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.35">
@@ -8192,7 +8189,7 @@
         <v>64</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>547</v>
@@ -8207,7 +8204,7 @@
         <v>548</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.35">
@@ -8221,7 +8218,7 @@
         <v>469</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>468</v>
@@ -8236,7 +8233,7 @@
         <v>471</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.35">
@@ -8250,7 +8247,7 @@
         <v>35</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>474</v>
@@ -8265,7 +8262,7 @@
         <v>475</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
@@ -8279,7 +8276,7 @@
         <v>35</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>474</v>
@@ -8294,7 +8291,7 @@
         <v>475</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
@@ -8308,7 +8305,7 @@
         <v>490</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E100" s="3" t="s">
         <v>493</v>
@@ -8323,10 +8320,10 @@
         <v>494</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
@@ -8340,7 +8337,7 @@
         <v>64</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>566</v>
@@ -8355,7 +8352,7 @@
         <v>567</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
@@ -8369,7 +8366,7 @@
         <v>469</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>465</v>
@@ -8384,7 +8381,7 @@
         <v>466</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
@@ -8398,7 +8395,7 @@
         <v>490</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>493</v>
@@ -8416,7 +8413,7 @@
         <v>492</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.35">
@@ -8427,10 +8424,10 @@
         <v>459</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>455</v>
@@ -8445,7 +8442,7 @@
         <v>457</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
@@ -8459,7 +8456,7 @@
         <v>35</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>412</v>
@@ -8474,7 +8471,7 @@
         <v>413</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
@@ -8485,10 +8482,10 @@
         <v>415</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>533</v>
@@ -8503,7 +8500,7 @@
         <v>534</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
@@ -8517,7 +8514,7 @@
         <v>64</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>303</v>
@@ -8535,7 +8532,7 @@
         <v>462</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.35">
@@ -8549,7 +8546,7 @@
         <v>35</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>517</v>
@@ -8567,7 +8564,7 @@
         <v>515</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
@@ -8581,7 +8578,7 @@
         <v>64</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>442</v>
@@ -8596,7 +8593,7 @@
         <v>443</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.35">
@@ -8610,7 +8607,7 @@
         <v>64</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>538</v>
@@ -8625,7 +8622,7 @@
         <v>539</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.35">
@@ -8639,7 +8636,7 @@
         <v>591</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>592</v>
@@ -8657,7 +8654,7 @@
         <v>588</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
@@ -8671,7 +8668,7 @@
         <v>64</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>303</v>
@@ -8689,7 +8686,7 @@
         <v>448</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
@@ -8703,7 +8700,7 @@
         <v>64</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>424</v>
@@ -8715,7 +8712,7 @@
         <v>423</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
@@ -8729,7 +8726,7 @@
         <v>35</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E114" s="3" t="s">
         <v>324</v>
@@ -8747,7 +8744,7 @@
         <v>483</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
@@ -8761,7 +8758,7 @@
         <v>64</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F115" s="3" t="s">
         <v>557</v>
@@ -8776,7 +8773,7 @@
         <v>558</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.35">
@@ -8787,10 +8784,10 @@
         <v>532</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F116" s="3" t="s">
         <v>529</v>
@@ -8805,7 +8802,7 @@
         <v>530</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.35">
@@ -8819,7 +8816,7 @@
         <v>35</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>406</v>
@@ -8837,7 +8834,7 @@
         <v>417</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
@@ -8851,7 +8848,7 @@
         <v>64</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F118" s="3" t="s">
         <v>420</v>
@@ -8866,7 +8863,7 @@
         <v>421</v>
       </c>
       <c r="J118" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
@@ -8880,7 +8877,7 @@
         <v>35</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>427</v>
@@ -8895,7 +8892,7 @@
         <v>429</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
@@ -8909,7 +8906,7 @@
         <v>64</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F120" s="3" t="s">
         <v>430</v>
@@ -8924,7 +8921,7 @@
         <v>432</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
@@ -8938,7 +8935,7 @@
         <v>35</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>324</v>
@@ -8956,7 +8953,7 @@
         <v>478</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.35">
@@ -8967,10 +8964,10 @@
         <v>12</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F122" s="3" t="s">
         <v>498</v>
@@ -8985,7 +8982,7 @@
         <v>499</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
@@ -8999,7 +8996,7 @@
         <v>64</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F123" s="3" t="s">
         <v>575</v>
@@ -9014,7 +9011,7 @@
         <v>576</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.35">
@@ -9028,7 +9025,7 @@
         <v>64</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>303</v>
@@ -9046,7 +9043,7 @@
         <v>454</v>
       </c>
       <c r="J124" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.35">
@@ -9060,7 +9057,7 @@
         <v>527</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>523</v>
@@ -9075,7 +9072,7 @@
         <v>524</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
@@ -9089,7 +9086,7 @@
         <v>64</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>571</v>
@@ -9104,7 +9101,7 @@
         <v>572</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.35">
@@ -9118,7 +9115,7 @@
         <v>64</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>579</v>
@@ -9133,7 +9130,7 @@
         <v>580</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.35">
@@ -9147,7 +9144,7 @@
         <v>35</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>583</v>
@@ -9162,7 +9159,7 @@
         <v>584</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
@@ -9176,7 +9173,7 @@
         <v>226</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F129" s="3" t="s">
         <v>485</v>
@@ -9191,7 +9188,7 @@
         <v>486</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.35">
@@ -9205,7 +9202,7 @@
         <v>35</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>434</v>
@@ -9220,7 +9217,7 @@
         <v>436</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.35">
@@ -9234,7 +9231,7 @@
         <v>64</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>439</v>
@@ -9249,7 +9246,7 @@
         <v>440</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.35">
@@ -9260,10 +9257,10 @@
         <v>564</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>561</v>
@@ -9278,7 +9275,7 @@
         <v>562</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.35">
@@ -9286,28 +9283,28 @@
         <v>2024</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F133" t="s">
+        <v>600</v>
+      </c>
+      <c r="G133" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="G133" s="3" t="s">
+      <c r="H133" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="H133" s="3" t="s">
-        <v>603</v>
-      </c>
       <c r="I133" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.35">
@@ -9321,22 +9318,22 @@
         <v>64</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="H134" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="I134" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="I134" s="3" t="s">
-        <v>607</v>
-      </c>
       <c r="J134" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.35">
@@ -9344,31 +9341,31 @@
         <v>2024</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>324</v>
       </c>
       <c r="F135" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="H135" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="G135" s="3" t="s">
+      <c r="I135" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="H135" s="3" t="s">
-        <v>611</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>613</v>
-      </c>
       <c r="J135" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.35">
@@ -9376,88 +9373,88 @@
         <v>2024</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D136" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="G136" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="F136" s="3" t="s">
-        <v>620</v>
-      </c>
-      <c r="G136" s="3" t="s">
+      <c r="H136" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="H136" s="3" t="s">
+      <c r="I136" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="I136" s="3" t="s">
-        <v>619</v>
-      </c>
       <c r="J136" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J137" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J138" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J139" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J140" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J141" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J142" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J143" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J144" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="145" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J145" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="146" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J146" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="147" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J147" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="148" spans="10:10" x14ac:dyDescent="0.35">
       <c r="J148" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>
@@ -9474,8 +9471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F627AA-E3AE-4351-92AE-68BECE4A1E4C}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9718,11 +9715,11 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="B29" s="3">
         <f>COUNTIF('Ringamp Publication List'!$C$2:$E$997,Analysis!A29)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -9736,7 +9733,7 @@
       </c>
       <c r="B32" s="3">
         <f>SUM(B18:B29)</f>
-        <v>109</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -9857,7 +9854,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B49" s="3">
         <f>COUNTA('Ringamp Publication List'!$A$2:$A$997)-SUM(B38:B48)</f>

</xml_diff>